<commit_message>
feat: add medcard import
</commit_message>
<xml_diff>
--- a/static/files/1.xlsx
+++ b/static/files/1.xlsx
@@ -1274,7 +1274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1295,40 +1295,35 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>vac_name</t>
+          <t>vac_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vac_type</t>
+          <t>vac_date</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>vac_date</t>
+          <t>serial</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>serial</t>
+          <t>dose</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>dose</t>
+          <t>introduction_method</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>introduction_method</t>
+          <t>reaction</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>reaction</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>doctor</t>
         </is>
@@ -1343,36 +1338,31 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Коклюш</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
           <t>Вакцинация I</t>
         </is>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="1" t="n">
         <v>45030</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>АА2548</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="F2" t="n">
         <v>15.2</v>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Пероральный</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Пероральный</t>
+          <t>Немедленная</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>Немедленная</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t>Иванов Иван Иванович</t>
         </is>

</xml_diff>